<commit_message>
fix bug on parsing json files and start removing console files
</commit_message>
<xml_diff>
--- a/Eco-Track/website/api/controllers/Products/products.xlsx
+++ b/Eco-Track/website/api/controllers/Products/products.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
-    <t xml:space="preserve">ID</t>
+    <t xml:space="preserve">id</t>
   </si>
   <si>
     <t xml:space="preserve">Eco-friendly</t>
@@ -174,7 +174,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>